<commit_message>
Separated larval and adult transcriptomes onto different sheets
</commit_message>
<xml_diff>
--- a/c_gigas_transcriptome_SRA_bioprojects_version2.xlsx
+++ b/c_gigas_transcriptome_SRA_bioprojects_version2.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28620" windowHeight="17520" tabRatio="500"/>
+    <workbookView xWindow="1000" yWindow="0" windowWidth="28720" windowHeight="16340" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Full_data" sheetId="1" r:id="rId1"/>
+    <sheet name="Adult_transcriptomes" sheetId="2" r:id="rId2"/>
+    <sheet name="Larvae transcriptomes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="128">
   <si>
     <t>Crassostrea gigas relevant Bioprojects:</t>
   </si>
@@ -521,7 +523,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -540,6 +542,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -590,7 +609,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -603,6 +622,23 @@
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -943,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1779,4 +1815,466 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="80.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="75">
+      <c r="A3" s="4">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75">
+      <c r="A4" s="4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="75">
+      <c r="A5" s="4">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="75">
+      <c r="A6" s="4">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75">
+      <c r="A7" s="4">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="75">
+      <c r="A8" s="4">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="75">
+      <c r="A9" s="4">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75">
+      <c r="A10" s="4">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="75">
+      <c r="A11" s="4">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="75">
+      <c r="A12" s="4">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="135">
+      <c r="A13" s="4">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75">
+      <c r="A4" s="4">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="90">
+      <c r="A5" s="4">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="165">
+      <c r="A6" s="4">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="180">
+      <c r="A7" s="4">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="75">
+      <c r="A8" s="4">
+        <v>35</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" tooltip="Collapse the text"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
created target file spreadsheet and added Accession numbers to old spreadsheet
</commit_message>
<xml_diff>
--- a/c_gigas_transcriptome_SRA_bioprojects_version2.xlsx
+++ b/c_gigas_transcriptome_SRA_bioprojects_version2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="0" windowWidth="28720" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="17120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Full_data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="161">
   <si>
     <t>Crassostrea gigas relevant Bioprojects:</t>
   </si>
@@ -405,13 +405,112 @@
   </si>
   <si>
     <t>WHOLE GENOMIC SEQUENCING</t>
+  </si>
+  <si>
+    <t>PRJNA353875</t>
+  </si>
+  <si>
+    <t>AccessionID</t>
+  </si>
+  <si>
+    <t>PRJNA316106</t>
+  </si>
+  <si>
+    <t>PRJNA316154</t>
+  </si>
+  <si>
+    <t>PRJNA301543</t>
+  </si>
+  <si>
+    <t>PRJNA298285</t>
+  </si>
+  <si>
+    <t>PRJNA291364</t>
+  </si>
+  <si>
+    <t>PRJNA290387</t>
+  </si>
+  <si>
+    <t>PRJNA282703</t>
+  </si>
+  <si>
+    <t>PRJNA281706</t>
+  </si>
+  <si>
+    <t>PRJEB6270</t>
+  </si>
+  <si>
+    <t>PRJNA233581</t>
+  </si>
+  <si>
+    <t>PRJNA243050</t>
+  </si>
+  <si>
+    <t>PRJNA233562 </t>
+  </si>
+  <si>
+    <t>PRJNA233528</t>
+  </si>
+  <si>
+    <t>PAPMs stimulation</t>
+  </si>
+  <si>
+    <t>PRJNA233418</t>
+  </si>
+  <si>
+    <t>PRJNA232944</t>
+  </si>
+  <si>
+    <t>PRJNA232734</t>
+  </si>
+  <si>
+    <t>PRJNA217698 </t>
+  </si>
+  <si>
+    <t>PRJNA217287</t>
+  </si>
+  <si>
+    <t>PRJNA216134</t>
+  </si>
+  <si>
+    <t>PRJNA196535 </t>
+  </si>
+  <si>
+    <t>PRJNA194084 </t>
+  </si>
+  <si>
+    <t>PRJNA194079</t>
+  </si>
+  <si>
+    <t>PRJNA185434</t>
+  </si>
+  <si>
+    <t>PRJNA182358 </t>
+  </si>
+  <si>
+    <t>PRJNA178077</t>
+  </si>
+  <si>
+    <t>PRJNA167099</t>
+  </si>
+  <si>
+    <t>PRJNA154617</t>
+  </si>
+  <si>
+    <t>PRJNA154615</t>
+  </si>
+  <si>
+    <t>PRJNA146329</t>
+  </si>
+  <si>
+    <t>PRJNA71219</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -479,13 +578,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -523,7 +633,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -563,8 +673,94 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -601,15 +797,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -639,6 +836,92 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -977,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:G34"/>
+    <sheetView tabSelected="1" topLeftCell="D26" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -994,12 +1277,12 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21">
+    <row r="1" spans="1:13" ht="21">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:13">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
@@ -1019,8 +1302,11 @@
       <c r="G4" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30">
+      <c r="H4" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="30">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1033,7 +1319,7 @@
       <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="22" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1042,10 +1328,13 @@
       <c r="G5" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="75">
+      <c r="H5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="75">
       <c r="A6" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
@@ -1056,7 +1345,7 @@
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="22" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1065,10 +1354,13 @@
       <c r="G6" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="30">
+      <c r="H6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30">
       <c r="A7" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
@@ -1079,7 +1371,7 @@
       <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="22" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1088,10 +1380,13 @@
       <c r="G7" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="30">
+      <c r="H7" s="23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30">
       <c r="A8" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
@@ -1102,7 +1397,7 @@
       <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="22" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1111,10 +1406,13 @@
       <c r="G8" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="30">
+      <c r="H8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30">
       <c r="A9" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
@@ -1125,7 +1423,7 @@
       <c r="D9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="22" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1134,10 +1432,14 @@
       <c r="G9" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="30">
+      <c r="H9" t="s">
+        <v>133</v>
+      </c>
+      <c r="M9" s="23"/>
+    </row>
+    <row r="10" spans="1:13" ht="30">
       <c r="A10" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
@@ -1148,7 +1450,7 @@
       <c r="D10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="22" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1157,10 +1459,13 @@
       <c r="G10" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="30">
+      <c r="H10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="30">
       <c r="A11" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>3</v>
@@ -1171,19 +1476,22 @@
       <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="22" t="s">
         <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>97</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30">
+        <v>101</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30">
       <c r="A12" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
@@ -1194,7 +1502,7 @@
       <c r="D12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="22" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1203,10 +1511,13 @@
       <c r="G12" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="30">
+      <c r="H12" s="23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30">
       <c r="A13" s="4">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>3</v>
@@ -1217,7 +1528,7 @@
       <c r="D13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -1226,10 +1537,13 @@
       <c r="G13" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="30">
+      <c r="H13" s="23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30">
       <c r="A14" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>3</v>
@@ -1240,7 +1554,7 @@
       <c r="D14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="22" t="s">
         <v>30</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1249,10 +1563,13 @@
       <c r="G14" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="30">
+      <c r="H14" s="23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="30">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>3</v>
@@ -1263,7 +1580,7 @@
       <c r="D15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="22" t="s">
         <v>32</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1272,10 +1589,13 @@
       <c r="G15" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="30">
+      <c r="H15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>3</v>
@@ -1286,7 +1606,7 @@
       <c r="D16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="22" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1295,10 +1615,13 @@
       <c r="G16" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="30">
+      <c r="H16" s="23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>3</v>
@@ -1309,7 +1632,7 @@
       <c r="D17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="22" t="s">
         <v>36</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1318,10 +1641,13 @@
       <c r="G17" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="30">
+      <c r="H17" s="23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30">
       <c r="A18" s="4">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>3</v>
@@ -1332,19 +1658,22 @@
       <c r="D18" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="22" t="s">
         <v>38</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30">
+        <v>143</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30">
       <c r="A19" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>3</v>
@@ -1355,7 +1684,7 @@
       <c r="D19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="22" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -1364,10 +1693,13 @@
       <c r="G19" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="30">
+      <c r="H19" s="23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30">
       <c r="A20" s="4">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>3</v>
@@ -1378,7 +1710,7 @@
       <c r="D20" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="22" t="s">
         <v>43</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -1387,10 +1719,13 @@
       <c r="G20" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="30">
+      <c r="H20" s="23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30">
       <c r="A21" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>3</v>
@@ -1401,7 +1736,7 @@
       <c r="D21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="22" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1410,10 +1745,13 @@
       <c r="G21" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="30">
+      <c r="H21" s="23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30">
       <c r="A22" s="4">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>3</v>
@@ -1424,7 +1762,7 @@
       <c r="D22" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="22" t="s">
         <v>49</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -1433,10 +1771,13 @@
       <c r="G22" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="30">
+      <c r="H22" s="23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30">
       <c r="A23" s="4">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>3</v>
@@ -1447,7 +1788,7 @@
       <c r="D23" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="22" t="s">
         <v>51</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -1456,10 +1797,13 @@
       <c r="G23" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="30">
+      <c r="H23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30">
       <c r="A24" s="4">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>3</v>
@@ -1470,7 +1814,7 @@
       <c r="D24" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="22" t="s">
         <v>52</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -1479,10 +1823,13 @@
       <c r="G24" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="75">
+      <c r="H24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="75">
       <c r="A25" s="4">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>3</v>
@@ -1493,7 +1840,7 @@
       <c r="D25" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="22" t="s">
         <v>55</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -1502,10 +1849,13 @@
       <c r="G25" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="30">
+      <c r="H25" s="23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30">
       <c r="A26" s="4">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>3</v>
@@ -1516,7 +1866,7 @@
       <c r="D26" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="22" t="s">
         <v>58</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -1525,10 +1875,13 @@
       <c r="G26" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" s="21" customFormat="1" ht="30">
-      <c r="A27" s="17">
-        <v>27</v>
+      <c r="H26" s="23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="20" customFormat="1" ht="30">
+      <c r="A27" s="4">
+        <v>23</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>3</v>
@@ -1539,19 +1892,22 @@
       <c r="D27" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="G27" s="21" t="s">
+      <c r="G27" s="20" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="30">
+      <c r="H27" s="23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30">
       <c r="A28" s="4">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>3</v>
@@ -1562,7 +1918,7 @@
       <c r="D28" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="22" t="s">
         <v>62</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1571,10 +1927,13 @@
       <c r="G28" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="30">
+      <c r="H28" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30">
       <c r="A29" s="4">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>3</v>
@@ -1585,7 +1944,7 @@
       <c r="D29" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="22" t="s">
         <v>64</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -1594,10 +1953,13 @@
       <c r="G29" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="30">
+      <c r="H29" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30">
       <c r="A30" s="4">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>3</v>
@@ -1608,7 +1970,7 @@
       <c r="D30" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="22" t="s">
         <v>67</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -1617,10 +1979,13 @@
       <c r="G30" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="30">
+      <c r="H30" s="23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30">
       <c r="A31" s="4">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>3</v>
@@ -1631,7 +1996,7 @@
       <c r="D31" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="22" t="s">
         <v>69</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -1640,10 +2005,13 @@
       <c r="G31" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="75">
+      <c r="H31" s="23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="75">
       <c r="A32" s="4">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>3</v>
@@ -1654,19 +2022,22 @@
       <c r="D32" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="21" t="s">
         <v>122</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="75">
+      <c r="H32" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="75">
       <c r="A33" s="4">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>3</v>
@@ -1677,7 +2048,7 @@
       <c r="D33" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="22" t="s">
         <v>75</v>
       </c>
       <c r="F33" s="1" t="s">
@@ -1686,10 +2057,13 @@
       <c r="G33" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="30">
+      <c r="H33" s="23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30">
       <c r="A34" s="4">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>3</v>
@@ -1700,7 +2074,7 @@
       <c r="D34" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="22" t="s">
         <v>77</v>
       </c>
       <c r="F34" s="1" t="s">
@@ -1709,10 +2083,13 @@
       <c r="G34" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="30">
+      <c r="H34" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30">
       <c r="A35" s="4">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>3</v>
@@ -1723,7 +2100,7 @@
       <c r="D35" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="22" t="s">
         <v>80</v>
       </c>
       <c r="F35" s="1" t="s">
@@ -1732,18 +2109,19 @@
       <c r="G35" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H35" s="23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="39" spans="1:8">
       <c r="B39" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8">
       <c r="B40" s="1" t="s">
         <v>3</v>
       </c>
@@ -1754,7 +2132,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="B41" s="1" t="s">
         <v>3</v>
       </c>
@@ -1765,12 +2143,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8">
       <c r="B44" s="15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8">
       <c r="B45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1784,12 +2162,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:8">
       <c r="A48" s="4" t="s">
         <v>3</v>
       </c>
@@ -1821,7 +2199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:G13"/>
     </sheetView>
   </sheetViews>
@@ -1830,6 +2208,7 @@
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="33.6640625" customWidth="1"/>
     <col min="4" max="4" width="80.5" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
@@ -2083,7 +2462,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="135">
+    <row r="13" spans="1:7" ht="75">
       <c r="A13" s="4">
         <v>33</v>
       </c>
@@ -2099,7 +2478,7 @@
       <c r="E13" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="21" t="s">
         <v>122</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -2213,7 +2592,7 @@
       <c r="E6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="21" t="s">
         <v>122</v>
       </c>
       <c r="G6" s="1" t="s">

</xml_diff>